<commit_message>
Add description in services page
</commit_message>
<xml_diff>
--- a/files/system/import-services-sample.xlsx
+++ b/files/system/import-services-sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Company</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
   </si>
   <si>
     <t xml:space="preserve">Ifestos Marine Works</t>
@@ -293,7 +296,7 @@
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -309,7 +312,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="11.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="18.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="11.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1007" min="12" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="29.99"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1007" min="13" style="2" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -345,6 +349,9 @@
       </c>
       <c r="K1" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="ALT1" s="0"/>
       <c r="ALU1" s="0"/>
@@ -366,37 +373,37 @@
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>

</xml_diff>